<commit_message>
Add excel mutilply array test
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/AIConfig.xlsx
+++ b/Unity/Assets/Config/Excel/AIConfig.xlsx
@@ -4,18 +4,31 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13500" tabRatio="809" activeTab="1"/>
+    <workbookView windowWidth="22635" windowHeight="10800" tabRatio="809" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AIConfig_1" sheetId="6" r:id="rId1"/>
     <sheet name="AIConfig_2" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>cs</t>
   </si>
@@ -56,6 +69,9 @@
     <t>NodeParams</t>
   </si>
   <si>
+    <t>NodeParams2</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
@@ -71,21 +87,33 @@
     <t>攻击</t>
   </si>
   <si>
+    <t>1,0,2</t>
+  </si>
+  <si>
+    <t>[[1,0,2],[2,2,3]]</t>
+  </si>
+  <si>
     <t>AI_XunLuo</t>
   </si>
   <si>
     <t>巡逻</t>
+  </si>
+  <si>
+    <t>1,0,3</t>
+  </si>
+  <si>
+    <t>[[1,0,2],[2,2,4]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -108,10 +136,57 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -123,17 +198,64 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -144,22 +266,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -167,25 +273,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,67 +282,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,6 +302,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -286,31 +338,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,49 +470,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,85 +482,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,30 +493,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -503,6 +507,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,26 +544,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -565,153 +558,188 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -726,52 +754,52 @@
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
     <cellStyle name="常规 2" xfId="49"/>
@@ -1043,13 +1071,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G3:G4"/>
+      <selection activeCell="H6" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="9.60833333333333" style="1" customWidth="1"/>
@@ -1058,10 +1086,11 @@
     <col min="6" max="6" width="23.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.25" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="19.375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" spans="1:8">
+    <row r="1" ht="16.5" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1072,8 +1101,9 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
-    <row r="2" ht="16.5" spans="1:8">
+    <row r="2" ht="16.5" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1084,8 +1114,9 @@
         <v>1</v>
       </c>
       <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
-    <row r="3" ht="16.5" spans="1:8">
+    <row r="3" ht="16.5" spans="1:9">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
@@ -1106,8 +1137,11 @@
       <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" ht="16.5" spans="1:8">
+    <row r="4" ht="16.5" spans="1:9">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
@@ -1128,30 +1162,36 @@
       <c r="H4" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" ht="16.5" spans="1:8">
+    <row r="5" ht="16.5" spans="1:9">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" ht="16.5" spans="3:7">
+    <row r="6" ht="16.5" spans="3:9">
       <c r="C6" s="2">
         <f>D6*100+E6</f>
         <v>101</v>
@@ -1163,13 +1203,19 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" ht="16.5" spans="3:7">
+    <row r="7" s="1" customFormat="1" ht="16.5" spans="3:9">
       <c r="C7" s="2">
         <f>D7*100+E7</f>
         <v>102</v>
@@ -1181,10 +1227,16 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1196,13 +1248,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="9.60833333333333" style="1" customWidth="1"/>
@@ -1211,10 +1263,11 @@
     <col min="6" max="6" width="23.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.25" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="19.375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" spans="1:8">
+    <row r="1" ht="16.5" spans="1:9">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1223,8 +1276,9 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
-    <row r="2" ht="16.5" spans="1:8">
+    <row r="2" ht="16.5" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1235,8 +1289,9 @@
         <v>1</v>
       </c>
       <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
-    <row r="3" ht="16.5" spans="1:8">
+    <row r="3" ht="16.5" spans="1:9">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
@@ -1257,8 +1312,11 @@
       <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" ht="16.5" spans="1:8">
+    <row r="4" ht="16.5" spans="1:9">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
@@ -1279,30 +1337,36 @@
       <c r="H4" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" ht="16.5" spans="1:8">
+    <row r="5" ht="16.5" spans="1:9">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" ht="16.5" spans="3:7">
+    <row r="6" ht="16.5" spans="3:9">
       <c r="C6" s="2">
         <f>D6*100+E6</f>
         <v>201</v>
@@ -1314,10 +1378,16 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>